<commit_message>
Modelo de dados OBM e Tabelas
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/DashboardImunizacao.xlsx
+++ b/Gestão do Projeto/Indicadores/DashboardImunizacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Gestão do Projeto/Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6C6C8B-0E1B-E64A-BE64-0465CCDB7593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25F126B-D592-0A4D-8001-170A566EEC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1000,8 +1000,8 @@
   </sheetPr>
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1011,9 +1011,10 @@
     <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="56.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.1640625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="12.5" hidden="1" customWidth="1"/>
+    <col min="11" max="14" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Apresentações IPS Abril 24
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/Indicadores/DashboardImunizacao.xlsx
+++ b/Gestão do Projeto/Indicadores/DashboardImunizacao.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Gestão do Projeto/Indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25F126B-D592-0A4D-8001-170A566EEC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB5D250-512D-9B48-89F1-C347DD0A4642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="1220" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tarefas" sheetId="1" r:id="rId1"/>
+    <sheet name="Março-23" sheetId="1" r:id="rId1"/>
+    <sheet name="Abril-23" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="49">
   <si>
     <t>Mapeamento semântico</t>
   </si>
@@ -797,6 +798,201 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="390525" cy="257175"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image3.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34DCB2FC-45D1-7441-8260-61B4000A79A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8728075" y="1085850"/>
+          <a:ext cx="390525" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="390525" cy="257175"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="image1.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F337C5B0-27E7-3147-8D5C-059D7A21C405}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="495300" y="1085850"/>
+          <a:ext cx="390525" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="447675" cy="257175"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="image2.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DCC5C9F-C220-B84F-968E-D8CF72EE0E67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5743575" y="1085850"/>
+          <a:ext cx="447675" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="390525" cy="257175"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="image1.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12FFA36C-A401-AC4C-A264-9D1DB80A508A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13131800" y="333375"/>
+          <a:ext cx="390525" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="390525" cy="257175"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="image3.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70BCE44D-4BF2-D144-9AE8-A258E60FEE8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13779500" y="323850"/>
+          <a:ext cx="390525" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1000,8 +1196,8 @@
   </sheetPr>
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1846,4 +2042,833 @@
   <pageSetup orientation="portrait" r:id="rId10"/>
   <drawing r:id="rId11"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7A3EE9-64F0-4745-978A-37E0D85C5C3B}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:T17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="56.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="33">
+        <f t="shared" ref="J2:S2" si="0">COUNTIF(J4:J17, "TRUE")/(COUNTIF(J4:J17, "TRUE")+COUNTIF(J4:J17, "FALSE"))</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L2" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M2" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N2" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O2" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P2" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q2" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R2" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S2" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T2" s="38">
+        <f>AVERAGE(T4:T17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="43" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" s="35">
+        <f>COUNTIF(J4:S4,"TRUE")/(COUNTIF(J4:S4,"TRUE")+COUNTIF(J4:S4,"FALSE"))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="S5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5" s="36">
+        <f t="shared" ref="T5:T15" si="1">COUNTIF(J5:S5,"TRUE")/(COUNTIF(J5:S5,"TRUE")+COUNTIF(J5:S5,"FALSE"))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="36"/>
+    </row>
+    <row r="7" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="36"/>
+    </row>
+    <row r="8" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="36"/>
+    </row>
+    <row r="9" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="36"/>
+    </row>
+    <row r="10" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="36"/>
+    </row>
+    <row r="11" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A11" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="36"/>
+    </row>
+    <row r="12" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A12" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="36"/>
+    </row>
+    <row r="13" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="36"/>
+    </row>
+    <row r="14" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="R14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="S14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T14" s="36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="R15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="S15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T15" s="36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="36"/>
+    </row>
+    <row r="17" spans="1:20" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="37"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="http://hl7.org/fhir/ValueSet/immunization-status" xr:uid="{1A42F002-C8E6-294C-B2A8-534288D5BEDB}"/>
+    <hyperlink ref="H4" location="'ConceptMapimmunization-status'!A1" display="ConceptMap/immunization-status" xr:uid="{BEE44659-5D9B-B749-A8E5-52C31989C338}"/>
+    <hyperlink ref="A5" r:id="rId2" display="http://hl7.org/fhir/uv/ips/ValueSet/vaccines-snomed-ct-ips-free-set" xr:uid="{8DB3F869-8221-CC47-AF97-A2C74507EEC4}"/>
+    <hyperlink ref="H5" location="'ConceptMapvaccine-code'!A1" display="ConceptMap/immunization-vaccine-code" xr:uid="{C7E83900-9C33-F746-AAAC-E931F40D7181}"/>
+    <hyperlink ref="A10" r:id="rId3" xr:uid="{F6F49F93-FCD9-934F-A274-D48DC8304C6B}"/>
+    <hyperlink ref="H10" location="'ConceptMapimmunization-report-o'!A1" display="ConceptMap/immunization-report-origin" xr:uid="{D80AFF4B-04DB-764E-8C5C-299A3AD5EB41}"/>
+    <hyperlink ref="A14" r:id="rId4" xr:uid="{8E361945-DDED-0043-B223-52D2CD7CA917}"/>
+    <hyperlink ref="G14" r:id="rId5" xr:uid="{018496AF-D6F6-7C4B-AAD2-E4D88DDBB110}"/>
+    <hyperlink ref="H14" location="'ConceptMapimmunization-site'!A1" display="ConceptMap/immunization-site" xr:uid="{25481952-0AAB-034B-ABB1-BAA8B79442FE}"/>
+    <hyperlink ref="A15" r:id="rId6" xr:uid="{64CDD131-C7AD-D646-A7B3-0BD6070E7163}"/>
+    <hyperlink ref="G15" r:id="rId7" xr:uid="{8821BBFF-85F6-3242-BC7A-E25204BD83B6}"/>
+    <hyperlink ref="H15" location="'ConceptMapimmunization-route'!A1" display="ConceptMap/immunization-route" xr:uid="{DAB23485-45F6-E442-985D-30980CFB63B5}"/>
+    <hyperlink ref="G4" r:id="rId8" display="http://www.saude.gov.br/fhir/r4/ValueSet/BREstadoEvento-1.0" xr:uid="{51D22F13-0990-6048-A537-59401F495E72}"/>
+    <hyperlink ref="G5" r:id="rId9" display="http://www.saude.gov.br/fhir/r4/ValueSet/BRImunobiologico-1.0" xr:uid="{E8D4900F-0D1C-8C4A-AE37-1A1EB4A218CF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+  <drawing r:id="rId11"/>
+</worksheet>
 </file>
</xml_diff>